<commit_message>
fix: updated neo4j test results
</commit_message>
<xml_diff>
--- a/test_results/VotiNeo4J.xlsx
+++ b/test_results/VotiNeo4J.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\DBMS NoSQL\FITSTIC_NoSQL_2025\test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50C1206-83B3-48FE-A2A2-859491E21B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A04EE5-0F50-48B6-91FB-25AEAE3A49D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>s.angelicchio@itsolivetti.it</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Voto</t>
+  </si>
+  <si>
+    <t>m.milasinovic@itsolivetti.it</t>
+  </si>
+  <si>
+    <t>g.biancoli@itsolivetti.it</t>
   </si>
 </sst>
 </file>
@@ -120,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -199,24 +205,76 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="medium">
         <color rgb="FFF8F9FA"/>
@@ -228,26 +286,24 @@
         <color indexed="64"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="medium">
         <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFF8F9FA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -257,9 +313,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -269,31 +324,50 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -574,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G22"/>
+  <dimension ref="C3:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,105 +659,124 @@
     <col min="3" max="3" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="11" t="s">
+    <row r="3" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="13" t="s">
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="3" t="s">
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="3" t="s">
+    <row r="9" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>82</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="3" t="s">
+    </row>
+    <row r="11" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>90</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="4" t="s">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="3" t="s">
+    <row r="13" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="4" t="s">
+    <row r="14" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="13">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="5" t="s">
+    <row r="15" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="15">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G22" s="10"/>
+    <row r="16" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G22" s="7"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="J26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>